<commit_message>
included section for XYZ and XY in BOM, incase people want to make only XY stages.
</commit_message>
<xml_diff>
--- a/Piezo-Nanopositioner-V1/CAD Design/MECH_piezo_stage_BOM.xlsx
+++ b/Piezo-Nanopositioner-V1/CAD Design/MECH_piezo_stage_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radur\Projects\Hacker Fab\Hardware\Piezo-Nanopositioner-V1\CAD Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82817F2-ACC2-47A9-ADA9-A100A35AC926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F72CEE4-83E3-4AB7-84F4-06166D6C4D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
   <si>
     <t>Part</t>
   </si>
@@ -69,20 +69,74 @@
     <t>Nut for Rail</t>
   </si>
   <si>
-    <t>Rail</t>
-  </si>
-  <si>
     <t>Linear Bearing</t>
   </si>
   <si>
     <t>1 (pack of 100)</t>
+  </si>
+  <si>
+    <t>RF SMA Male to SMA Male Cable 2FT</t>
+  </si>
+  <si>
+    <t>https://www.amazon.ca/XRDS-RF-Coaxial-Extension-Antenna/dp/B0C4TGWGM2?dib=undefined&amp;th=1</t>
+  </si>
+  <si>
+    <t>RF2-145A-T-17-50-G-HDW</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/adam-tech/RF2-145A-T-17-50-G-HDW/9831202</t>
+  </si>
+  <si>
+    <t>Black-Oxide, M6 x 1 mm Thread, 16 mm Long</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/91290A321/</t>
+  </si>
+  <si>
+    <t>Screw for Optical Breadboard</t>
+  </si>
+  <si>
+    <t>Male-2-male SMA Cable</t>
+  </si>
+  <si>
+    <t>Female SMA Connector</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>2 (packages of 2)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rail - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SELECT RAIL LENGTH OF 60MM</t>
+    </r>
+  </si>
+  <si>
+    <t>For XYZ Stage</t>
+  </si>
+  <si>
+    <t>For XY Stage</t>
+  </si>
+  <si>
+    <t>1 (packages of 2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,8 +158,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,12 +189,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -133,16 +208,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -424,94 +532,292 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E6"/>
+  <dimension ref="B2:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="61.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="94.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="8">
+        <v>3</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="8">
+        <v>3</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="9">
+        <v>3</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="12">
+        <v>5</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C17" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="8">
+        <v>2</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="8">
+        <v>2</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2">
-        <v>3</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2">
-        <v>3</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
+      <c r="C20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="9">
+        <v>2</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="12">
+        <v>5</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B14:E14"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{C8E24F93-2F39-4EF7-9EBA-96951FF60006}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{0F5CFEEC-802C-4268-A36D-9D6D921CFCE1}"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{C8E24F93-2F39-4EF7-9EBA-96951FF60006}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{0F5CFEEC-802C-4268-A36D-9D6D921CFCE1}"/>
+    <hyperlink ref="C8" r:id="rId3" xr:uid="{8176881E-1A58-42DD-8AFE-7EE901D86DD5}"/>
+    <hyperlink ref="C9" r:id="rId4" xr:uid="{BB2CE9A3-01A2-4EF8-94F2-A78CB732B514}"/>
+    <hyperlink ref="C10" r:id="rId5" xr:uid="{C3E8798C-19B0-49FC-8ACE-DDA12093E198}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{92352C86-429A-4086-A1E4-035A59D49C04}"/>
+    <hyperlink ref="C6" r:id="rId7" xr:uid="{BE4A2203-17FF-481F-9950-5136E7C0E456}"/>
+    <hyperlink ref="C16" r:id="rId8" xr:uid="{BB57C7A4-0153-496F-B867-CC98F8D6C82D}"/>
+    <hyperlink ref="C17" r:id="rId9" xr:uid="{4C5F6976-DA79-43EE-A7E2-80716567A96D}"/>
+    <hyperlink ref="C20" r:id="rId10" xr:uid="{1F732145-6DA1-42E1-A2CA-4CF1D71418F8}"/>
+    <hyperlink ref="C21" r:id="rId11" xr:uid="{3AA877E9-3868-43BA-8CE3-345B9D51D120}"/>
+    <hyperlink ref="C22" r:id="rId12" xr:uid="{7092C846-EB72-491C-8B79-6F56F614CB5A}"/>
+    <hyperlink ref="C19" r:id="rId13" xr:uid="{C2C9E83E-DD32-4B82-AF15-B0E7B96E0E6B}"/>
+    <hyperlink ref="C18" r:id="rId14" xr:uid="{E5B9A21D-0F4D-4391-9B26-E9780D998BF6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>